<commit_message>
Fixed an error with some chartacters not included in reg exp. Added a parametrized unit test for data extraction.
</commit_message>
<xml_diff>
--- a/fn_utilities/tests/data/excel_query/budget.xlsx
+++ b/fn_utilities/tests/data/excel_query/budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihor.Husar@ibm.com/resilient/testing_openpyxl/test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihor.Husar@ibm.com/resilient/resilient-community-apps/fn_utilities/tests/data/excel_query/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCA1A9-FCCB-E842-88BC-763EC0FEF772}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37088BA6-D99E-2B44-B2BE-68751E695F5E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN 2015" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="50">
   <si>
     <t>PLEASE STOP "REQUEST ACCESS"- Go To "File" -&gt; Make A Copy. I can't give you access, this is just a template.</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>October 2015</t>
+  </si>
+  <si>
+    <t>""''</t>
   </si>
 </sst>
 </file>
@@ -508,8 +511,33 @@
     <xf numFmtId="165" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="14" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -525,31 +553,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,7 +1066,7 @@
   </sheetPr>
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -1077,7 +1080,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="38"/>
@@ -1114,7 +1117,7 @@
         <v>42035</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -1140,15 +1143,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -1166,7 +1169,7 @@
       <c r="F5" s="9">
         <v>300</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -1184,7 +1187,7 @@
       <c r="F6" s="9">
         <v>30</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -1208,13 +1211,13 @@
       <c r="F8" s="9">
         <v>70</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
@@ -1225,9 +1228,9 @@
       <c r="F9" s="9">
         <v>50</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
@@ -1238,40 +1241,40 @@
       <c r="F10" s="9">
         <v>20</v>
       </c>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -1289,17 +1292,17 @@
         <f>SUM(F5:F13)</f>
         <v>520</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>100</v>
       </c>
@@ -1313,12 +1316,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>3.225806451612903</v>
       </c>
@@ -1332,7 +1335,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -1462,7 +1465,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-17.596774193548388</v>
       </c>
-      <c r="G25" s="57" t="s">
+      <c r="G25" s="37" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="22">
@@ -2200,10 +2203,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>96</v>
@@ -2219,11 +2222,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G25:G30"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B18:D19"/>
-    <mergeCell ref="B16:D17"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
@@ -2237,6 +2235,11 @@
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="G25:G30"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B18:D19"/>
+    <mergeCell ref="B16:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThanOrEqual">
@@ -2289,7 +2292,7 @@
         <v>42277</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -2315,15 +2318,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -2333,7 +2336,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -2343,7 +2346,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -2359,62 +2362,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -2432,17 +2435,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -2456,12 +2459,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -2475,7 +2478,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -3310,10 +3313,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -3397,7 +3400,7 @@
         <v>42308</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -3423,15 +3426,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -3441,7 +3444,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -3451,7 +3454,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -3467,62 +3470,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -3540,17 +3543,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -3564,12 +3567,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -3583,7 +3586,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -4418,10 +4421,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -4437,18 +4440,18 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="H8:H10"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="H8:H10"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B16:D17"/>
@@ -4505,7 +4508,7 @@
         <v>42338</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -4531,15 +4534,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -4549,7 +4552,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -4559,7 +4562,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -4575,62 +4578,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -4648,17 +4651,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -4672,12 +4675,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -4691,7 +4694,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -5526,10 +5529,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -5613,7 +5616,7 @@
         <v>42369</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -5639,15 +5642,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -5657,7 +5660,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -5667,7 +5670,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -5683,62 +5686,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -5756,17 +5759,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -5780,12 +5783,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -5799,7 +5802,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -6634,10 +6637,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -6653,6 +6656,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="B53:C53"/>
@@ -6663,12 +6672,6 @@
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6688,10 +6691,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D8EF9C-FE92-DE42-8F65-6A896CD97F2B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6733,7 +6744,7 @@
         <v>42063</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -6759,15 +6770,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -6777,7 +6788,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -6787,7 +6798,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -6803,62 +6814,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -6876,17 +6887,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -6900,12 +6911,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -6919,7 +6930,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -7754,10 +7765,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -7773,13 +7784,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B53:C53"/>
@@ -7789,6 +7793,13 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThanOrEqual">
@@ -7841,7 +7852,7 @@
         <v>42094</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -7867,15 +7878,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -7885,7 +7896,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -7895,7 +7906,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -7911,62 +7922,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -7984,17 +7995,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -8008,12 +8019,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -8027,7 +8038,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -8862,10 +8873,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -8881,6 +8892,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
@@ -8890,13 +8908,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThanOrEqual">
@@ -8949,7 +8960,7 @@
         <v>42124</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -8975,15 +8986,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -8993,7 +9004,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -9003,7 +9014,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -9019,62 +9030,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -9092,17 +9103,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -9116,12 +9127,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -9135,7 +9146,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -9970,10 +9981,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -9989,22 +10000,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B16:D17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="E18:F19"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B16:D17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThanOrEqual">
@@ -10057,7 +10068,7 @@
         <v>42155</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -10083,15 +10094,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -10101,7 +10112,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -10111,7 +10122,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -10127,62 +10138,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -10200,17 +10211,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -10224,12 +10235,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -10243,7 +10254,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -11078,10 +11089,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -11097,6 +11108,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I20:J20"/>
@@ -11108,11 +11124,6 @@
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThanOrEqual">
@@ -11165,7 +11176,7 @@
         <v>42185</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -11191,15 +11202,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -11209,7 +11220,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -11219,7 +11230,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -11235,62 +11246,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -11308,17 +11319,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -11332,12 +11343,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -11351,7 +11362,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -12186,10 +12197,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -12273,7 +12284,7 @@
         <v>42216</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -12299,15 +12310,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -12317,7 +12328,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -12327,7 +12338,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -12343,62 +12354,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -12416,17 +12427,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -12440,12 +12451,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -12459,7 +12470,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -13294,10 +13305,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -13313,11 +13324,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="I20:J20"/>
@@ -13329,6 +13335,11 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThanOrEqual">
@@ -13381,7 +13392,7 @@
         <v>42247</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -13407,15 +13418,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="50" t="s">
+      <c r="C4" s="41"/>
+      <c r="E4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="H4" s="52" t="s">
+      <c r="F4" s="41"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -13425,7 +13436,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -13435,7 +13446,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -13451,62 +13462,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="54"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -13524,17 +13535,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="56">
+      <c r="E16" s="39">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -13548,12 +13559,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="56">
+      <c r="E18" s="39">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -13567,7 +13578,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="43" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -14402,10 +14413,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="51"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Added E2E tests with mocked responses, and more unit tests for named ranges. All tests pass.
</commit_message>
<xml_diff>
--- a/fn_utilities/tests/data/excel_query/budget.xlsx
+++ b/fn_utilities/tests/data/excel_query/budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihor.Husar@ibm.com/resilient/resilient-community-apps/fn_utilities/tests/data/excel_query/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37088BA6-D99E-2B44-B2BE-68751E695F5E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DA7B85-82BC-644D-BB11-A6C7CAD8E417}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="920" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN 2015" sheetId="1" r:id="rId1"/>
@@ -511,24 +511,12 @@
     <xf numFmtId="165" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="14" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -536,6 +524,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -553,6 +544,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1080,7 +1080,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="38"/>
@@ -1117,7 +1117,7 @@
         <v>42035</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -1143,15 +1143,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -1169,7 +1169,7 @@
       <c r="F5" s="9">
         <v>300</v>
       </c>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -1187,7 +1187,7 @@
       <c r="F6" s="9">
         <v>30</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -1211,13 +1211,13 @@
       <c r="F8" s="9">
         <v>70</v>
       </c>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
@@ -1228,9 +1228,9 @@
       <c r="F9" s="9">
         <v>50</v>
       </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
@@ -1241,40 +1241,40 @@
       <c r="F10" s="9">
         <v>20</v>
       </c>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -1292,17 +1292,17 @@
         <f>SUM(F5:F13)</f>
         <v>520</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>100</v>
       </c>
@@ -1316,12 +1316,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>3.225806451612903</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -1465,7 +1465,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-17.596774193548388</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="57" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="22">
@@ -2203,10 +2203,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>96</v>
@@ -2222,6 +2222,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G25:G30"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B18:D19"/>
+    <mergeCell ref="B16:D17"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
@@ -2235,11 +2240,6 @@
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="G25:G30"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B18:D19"/>
-    <mergeCell ref="B16:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThanOrEqual">
@@ -2292,7 +2292,7 @@
         <v>42277</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -2318,15 +2318,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -2336,7 +2336,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -2346,7 +2346,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -2362,62 +2362,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -2435,17 +2435,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -2459,12 +2459,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -3313,10 +3313,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -3400,7 +3400,7 @@
         <v>42308</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -3426,15 +3426,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -3444,7 +3444,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -3454,7 +3454,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -3470,62 +3470,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -3543,17 +3543,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -3567,12 +3567,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -3586,7 +3586,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -4421,10 +4421,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -4440,12 +4440,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="H8:H10"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
@@ -4456,6 +4450,12 @@
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
@@ -4508,7 +4508,7 @@
         <v>42338</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -4534,15 +4534,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -4552,7 +4552,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -4562,7 +4562,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -4578,62 +4578,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -4651,17 +4651,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -4675,12 +4675,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -5529,10 +5529,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -5616,7 +5616,7 @@
         <v>42369</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -5642,15 +5642,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -5660,7 +5660,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -5670,7 +5670,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -5686,62 +5686,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -5759,17 +5759,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -5783,12 +5783,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -5802,7 +5802,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -6637,10 +6637,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -6656,12 +6656,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="B53:C53"/>
@@ -6672,6 +6666,12 @@
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6744,7 +6744,7 @@
         <v>42063</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -6770,15 +6770,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -6788,7 +6788,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -6798,7 +6798,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -6814,62 +6814,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -6887,17 +6887,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -6911,12 +6911,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -6930,7 +6930,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -7765,10 +7765,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -7784,6 +7784,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B53:C53"/>
@@ -7793,13 +7800,6 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThanOrEqual">
@@ -7852,7 +7852,7 @@
         <v>42094</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -7878,15 +7878,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -7896,7 +7896,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -7906,7 +7906,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -7922,62 +7922,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -7995,17 +7995,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -8019,12 +8019,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -8038,7 +8038,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -8873,10 +8873,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -8892,13 +8892,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
@@ -8908,6 +8901,13 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThanOrEqual">
@@ -8960,7 +8960,7 @@
         <v>42124</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -8986,15 +8986,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -9004,7 +9004,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -9014,7 +9014,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -9030,62 +9030,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -9103,17 +9103,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -9127,12 +9127,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -9146,7 +9146,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -9981,10 +9981,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -10000,22 +10000,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B16:D17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="E18:F19"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B16:D17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThanOrEqual">
@@ -10068,7 +10068,7 @@
         <v>42155</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -10094,15 +10094,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -10112,7 +10112,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -10122,7 +10122,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -10138,62 +10138,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -10211,17 +10211,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -10235,12 +10235,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -10254,7 +10254,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -11089,10 +11089,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -11108,11 +11108,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I20:J20"/>
@@ -11124,6 +11119,11 @@
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThanOrEqual">
@@ -11176,7 +11176,7 @@
         <v>42185</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -11202,15 +11202,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -11220,7 +11220,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -11230,7 +11230,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -11246,62 +11246,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -11319,17 +11319,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -11343,12 +11343,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -11362,7 +11362,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -12197,10 +12197,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -12284,7 +12284,7 @@
         <v>42216</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -12310,15 +12310,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -12328,7 +12328,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -12338,7 +12338,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -12354,62 +12354,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -12427,17 +12427,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -12451,12 +12451,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -12470,7 +12470,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -13305,10 +13305,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -13324,6 +13324,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="I20:J20"/>
@@ -13335,11 +13340,6 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThanOrEqual">
@@ -13392,7 +13392,7 @@
         <v>42247</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="38"/>
@@ -13418,15 +13418,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="E4" s="44" t="s">
+      <c r="C4" s="40"/>
+      <c r="E4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="H4" s="45" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="38"/>
@@ -13436,7 +13436,7 @@
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="46" t="s">
+      <c r="H5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="38"/>
@@ -13446,7 +13446,7 @@
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="38"/>
@@ -13462,62 +13462,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -13535,17 +13535,17 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="59" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
-      <c r="E16" s="39">
+      <c r="E16" s="45">
         <f>C14-F14</f>
         <v>0</v>
       </c>
@@ -13559,12 +13559,12 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="39">
+      <c r="E18" s="45">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
@@ -13578,7 +13578,7 @@
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="37" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="38"/>
@@ -14413,10 +14413,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Fixed tests so they work for both Python 2 and 3. Added additional E2E and unit tests to complete code coverage.
</commit_message>
<xml_diff>
--- a/fn_utilities/tests/data/excel_query/budget.xlsx
+++ b/fn_utilities/tests/data/excel_query/budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihor.Husar@ibm.com/resilient/resilient-community-apps/fn_utilities/tests/data/excel_query/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DA7B85-82BC-644D-BB11-A6C7CAD8E417}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5747AB-7E74-BC48-AA66-F1E53E18A6DD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="920" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="920" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN 2015" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="51">
   <si>
     <t>PLEASE STOP "REQUEST ACCESS"- Go To "File" -&gt; Make A Copy. I can't give you access, this is just a template.</t>
   </si>
@@ -184,7 +184,10 @@
     <t>October 2015</t>
   </si>
   <si>
-    <t>""''</t>
+    <t>""''Ť</t>
+  </si>
+  <si>
+    <t>Ť</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -511,12 +514,25 @@
     <xf numFmtId="165" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="14" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,9 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,15 +557,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1066,8 +1070,8 @@
   </sheetPr>
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1080,23 +1084,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="A1" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1117,13 +1124,13 @@
         <v>42035</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -1143,18 +1150,18 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
@@ -1169,10 +1176,10 @@
       <c r="F5" s="9">
         <v>300</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B6" s="7" t="s">
@@ -1187,10 +1194,10 @@
       <c r="F6" s="9">
         <v>30</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -1211,13 +1218,13 @@
       <c r="F8" s="9">
         <v>70</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
@@ -1228,9 +1235,9 @@
       <c r="F9" s="9">
         <v>50</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
@@ -1241,40 +1248,40 @@
       <c r="F10" s="9">
         <v>20</v>
       </c>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -1292,53 +1299,53 @@
         <f>SUM(F5:F13)</f>
         <v>520</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>100</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>3.225806451612903</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -1465,7 +1472,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-17.596774193548388</v>
       </c>
-      <c r="G25" s="57" t="s">
+      <c r="G25" s="38" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="22">
@@ -1496,7 +1503,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-14.370967741935484</v>
       </c>
-      <c r="G26" s="38"/>
+      <c r="G26" s="39"/>
       <c r="I26" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42009</v>
@@ -1525,7 +1532,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-11.14516129032258</v>
       </c>
-      <c r="G27" s="38"/>
+      <c r="G27" s="39"/>
       <c r="I27" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42010</v>
@@ -1552,7 +1559,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-7.919354838709677</v>
       </c>
-      <c r="G28" s="38"/>
+      <c r="G28" s="39"/>
       <c r="I28" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42011</v>
@@ -1579,7 +1586,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-4.693548387096774</v>
       </c>
-      <c r="G29" s="38"/>
+      <c r="G29" s="39"/>
       <c r="I29" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42012</v>
@@ -1606,7 +1613,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>-1.467741935483871</v>
       </c>
-      <c r="G30" s="38"/>
+      <c r="G30" s="39"/>
       <c r="I30" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42013</v>
@@ -2203,10 +2210,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>96</v>
@@ -2222,11 +2229,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G25:G30"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B18:D19"/>
-    <mergeCell ref="B16:D17"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
@@ -2240,6 +2242,11 @@
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="G25:G30"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B18:D19"/>
+    <mergeCell ref="B16:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThanOrEqual">
@@ -2292,13 +2299,13 @@
         <v>42277</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -2318,38 +2325,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -2362,62 +2369,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -2435,53 +2442,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -3313,10 +3320,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -3400,13 +3407,13 @@
         <v>42308</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -3426,38 +3433,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -3470,62 +3477,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -3543,53 +3550,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -4421,10 +4428,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -4440,6 +4447,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="H8:H10"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
@@ -4450,12 +4463,6 @@
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
@@ -4508,13 +4515,13 @@
         <v>42338</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -4534,38 +4541,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -4578,62 +4585,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -4651,53 +4658,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -5529,10 +5536,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -5616,13 +5623,13 @@
         <v>42369</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -5642,38 +5649,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -5686,62 +5693,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -5759,53 +5766,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -6637,10 +6644,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -6656,6 +6663,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="B53:C53"/>
@@ -6666,12 +6679,6 @@
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6691,8 +6698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D8EF9C-FE92-DE42-8F65-6A896CD97F2B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6714,7 +6721,7 @@
   </sheetPr>
   <dimension ref="A2:Z53"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6744,13 +6751,13 @@
         <v>42063</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -6770,38 +6777,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -6814,62 +6821,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -6887,53 +6894,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -7765,10 +7772,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -7784,13 +7791,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B53:C53"/>
@@ -7800,6 +7800,13 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThanOrEqual">
@@ -7852,13 +7859,13 @@
         <v>42094</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -7878,38 +7885,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -7922,62 +7929,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -7995,53 +8002,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -8873,10 +8880,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -8892,6 +8899,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
@@ -8901,13 +8915,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThanOrEqual">
@@ -8960,13 +8967,13 @@
         <v>42124</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -8986,38 +8993,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -9030,62 +9037,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -9103,53 +9110,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -9981,10 +9988,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -10000,22 +10007,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B16:D17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="E18:F19"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B16:D17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThanOrEqual">
@@ -10068,13 +10075,13 @@
         <v>42155</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -10094,38 +10101,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -10138,62 +10145,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -10211,53 +10218,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -11089,10 +11096,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -11108,6 +11115,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I20:J20"/>
@@ -11119,11 +11131,6 @@
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThanOrEqual">
@@ -11176,13 +11183,13 @@
         <v>42185</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -11202,38 +11209,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -11246,62 +11253,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -11319,53 +11326,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -12197,10 +12204,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -12284,13 +12291,13 @@
         <v>42216</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -12310,38 +12317,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -12354,62 +12361,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -12427,53 +12434,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -13305,10 +13312,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -13324,11 +13331,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="I20:J20"/>
@@ -13340,6 +13342,11 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThanOrEqual">
@@ -13392,13 +13399,13 @@
         <v>42247</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -13418,38 +13425,38 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="H4" s="41" t="s">
+      <c r="F4" s="42"/>
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -13462,62 +13469,62 @@
       <c r="C8" s="11"/>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="E10" s="7"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12" t="s">
@@ -13535,53 +13542,53 @@
         <f>SUM(F5:F13)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="49"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="45">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="45">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="38"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -14413,10 +14420,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Added documentation. Removed string from binary. Added excel query to codegen. Added additional tests for types and more complex inputs.
</commit_message>
<xml_diff>
--- a/fn_utilities/tests/data/excel_query/budget.xlsx
+++ b/fn_utilities/tests/data/excel_query/budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihor.Husar@ibm.com/resilient/resilient-community-apps/fn_utilities/tests/data/excel_query/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5747AB-7E74-BC48-AA66-F1E53E18A6DD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE85CBEA-9616-0049-8B2A-4DE201219B6B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="920" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="19200" windowHeight="20220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN 2015" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="54">
   <si>
     <t>PLEASE STOP "REQUEST ACCESS"- Go To "File" -&gt; Make A Copy. I can't give you access, this is just a template.</t>
   </si>
@@ -189,12 +189,22 @@
   <si>
     <t>Ť</t>
   </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>A,4,A</t>
+  </si>
+  <si>
+    <t>[1,2,3]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -466,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -515,24 +525,15 @@
     <xf numFmtId="165" fontId="14" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -540,6 +541,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -557,6 +561,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1070,8 +1083,8 @@
   </sheetPr>
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1087,23 +1100,23 @@
       <c r="A1" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1124,13 +1137,13 @@
         <v>42035</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -1150,18 +1163,18 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
@@ -1176,10 +1189,10 @@
       <c r="F5" s="9">
         <v>300</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B6" s="7" t="s">
@@ -1197,7 +1210,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -1304,48 +1317,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>100</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>3.225806451612903</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -1371,10 +1384,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="14" x14ac:dyDescent="0.15">
-      <c r="B22" s="17">
-        <f t="shared" ref="B22:B52" ca="1" si="0">IF(INDIRECT(ADDRESS(ROW(), COLUMN()+8)),INDIRECT(ADDRESS(ROW(), COLUMN()+7)), )</f>
-        <v>42005</v>
-      </c>
+      <c r="B22" s="17"/>
       <c r="C22" s="18"/>
       <c r="D22" s="19">
         <v>0</v>
@@ -1384,7 +1394,7 @@
         <v>3.225806451612903</v>
       </c>
       <c r="F22" s="21">
-        <f t="shared" ref="F22:F52" ca="1" si="1">INDIRECT(ADDRESS(ROW(), COLUMN()-1))-INDIRECT(ADDRESS(ROW(), COLUMN()-2))</f>
+        <f t="shared" ref="F22:F52" ca="1" si="0">INDIRECT(ADDRESS(ROW(), COLUMN()-1))-INDIRECT(ADDRESS(ROW(), COLUMN()-2))</f>
         <v>3.225806451612903</v>
       </c>
       <c r="I22" s="22">
@@ -1398,7 +1408,7 @@
     </row>
     <row r="23" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="B23:B52" ca="1" si="1">IF(INDIRECT(ADDRESS(ROW(), COLUMN()+8)),INDIRECT(ADDRESS(ROW(), COLUMN()+7)), )</f>
         <v>42006</v>
       </c>
       <c r="C23" s="25" t="s">
@@ -1412,7 +1422,7 @@
         <v>6.4516129032258061</v>
       </c>
       <c r="F23" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.95161290322580605</v>
       </c>
       <c r="I23" s="22">
@@ -1426,7 +1436,7 @@
     </row>
     <row r="24" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B24" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42007</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -1440,7 +1450,7 @@
         <v>4.1774193548387091</v>
       </c>
       <c r="F24" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-20.822580645161292</v>
       </c>
       <c r="G24" s="28" t="s">
@@ -1457,7 +1467,7 @@
     </row>
     <row r="25" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B25" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42008</v>
       </c>
       <c r="C25" s="18"/>
@@ -1469,10 +1479,10 @@
         <v>-17.596774193548388</v>
       </c>
       <c r="F25" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-17.596774193548388</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="61" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="22">
@@ -1486,7 +1496,7 @@
     </row>
     <row r="26" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B26" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42009</v>
       </c>
       <c r="C26" s="25" t="s">
@@ -1500,10 +1510,10 @@
         <v>-14.370967741935484</v>
       </c>
       <c r="F26" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-14.370967741935484</v>
       </c>
-      <c r="G26" s="39"/>
+      <c r="G26" s="42"/>
       <c r="I26" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42009</v>
@@ -1515,7 +1525,7 @@
     </row>
     <row r="27" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B27" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42010</v>
       </c>
       <c r="C27" s="25" t="s">
@@ -1529,10 +1539,10 @@
         <v>-11.14516129032258</v>
       </c>
       <c r="F27" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-11.14516129032258</v>
       </c>
-      <c r="G27" s="39"/>
+      <c r="G27" s="42"/>
       <c r="I27" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42010</v>
@@ -1544,7 +1554,7 @@
     </row>
     <row r="28" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B28" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42011</v>
       </c>
       <c r="C28" s="18"/>
@@ -1556,10 +1566,10 @@
         <v>-7.919354838709677</v>
       </c>
       <c r="F28" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-7.919354838709677</v>
       </c>
-      <c r="G28" s="39"/>
+      <c r="G28" s="42"/>
       <c r="I28" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42011</v>
@@ -1571,7 +1581,7 @@
     </row>
     <row r="29" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B29" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42012</v>
       </c>
       <c r="C29" s="18"/>
@@ -1583,10 +1593,10 @@
         <v>-4.693548387096774</v>
       </c>
       <c r="F29" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-4.693548387096774</v>
       </c>
-      <c r="G29" s="39"/>
+      <c r="G29" s="42"/>
       <c r="I29" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42012</v>
@@ -1598,7 +1608,7 @@
     </row>
     <row r="30" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B30" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42013</v>
       </c>
       <c r="C30" s="18"/>
@@ -1610,10 +1620,10 @@
         <v>-1.467741935483871</v>
       </c>
       <c r="F30" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-1.467741935483871</v>
       </c>
-      <c r="G30" s="39"/>
+      <c r="G30" s="42"/>
       <c r="I30" s="22">
         <f t="shared" ca="1" si="2"/>
         <v>42013</v>
@@ -1625,7 +1635,7 @@
     </row>
     <row r="31" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B31" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42014</v>
       </c>
       <c r="C31" s="25" t="s">
@@ -1639,7 +1649,7 @@
         <v>1.758064516129032</v>
       </c>
       <c r="F31" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.75806451612903203</v>
       </c>
       <c r="G31" s="28" t="s">
@@ -1656,7 +1666,7 @@
     </row>
     <row r="32" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B32" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42015</v>
       </c>
       <c r="C32" s="18"/>
@@ -1668,7 +1678,7 @@
         <v>3.9838709677419351</v>
       </c>
       <c r="F32" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>3.9838709677419351</v>
       </c>
       <c r="I32" s="22">
@@ -1682,7 +1692,7 @@
     </row>
     <row r="33" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B33" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42016</v>
       </c>
       <c r="C33" s="18"/>
@@ -1694,7 +1704,7 @@
         <v>7.2096774193548381</v>
       </c>
       <c r="F33" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>7.2096774193548381</v>
       </c>
       <c r="I33" s="22">
@@ -1708,7 +1718,7 @@
     </row>
     <row r="34" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B34" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42017</v>
       </c>
       <c r="C34" s="18"/>
@@ -1720,7 +1730,7 @@
         <v>10.43548387096774</v>
       </c>
       <c r="F34" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>10.43548387096774</v>
       </c>
       <c r="I34" s="22">
@@ -1734,7 +1744,7 @@
     </row>
     <row r="35" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B35" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42018</v>
       </c>
       <c r="C35" s="18"/>
@@ -1746,7 +1756,7 @@
         <v>13.661290322580644</v>
       </c>
       <c r="F35" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>13.661290322580644</v>
       </c>
       <c r="I35" s="22">
@@ -1760,7 +1770,7 @@
     </row>
     <row r="36" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B36" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42019</v>
       </c>
       <c r="C36" s="18"/>
@@ -1772,7 +1782,7 @@
         <v>16.887096774193548</v>
       </c>
       <c r="F36" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>16.887096774193548</v>
       </c>
       <c r="I36" s="22">
@@ -1786,7 +1796,7 @@
     </row>
     <row r="37" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B37" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42020</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -1800,7 +1810,7 @@
         <v>20.112903225806452</v>
       </c>
       <c r="F37" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>14.612903225806452</v>
       </c>
       <c r="I37" s="22">
@@ -1814,7 +1824,7 @@
     </row>
     <row r="38" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B38" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42021</v>
       </c>
       <c r="C38" s="18"/>
@@ -1826,7 +1836,7 @@
         <v>17.838709677419356</v>
       </c>
       <c r="F38" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>17.838709677419356</v>
       </c>
       <c r="I38" s="22">
@@ -1840,7 +1850,7 @@
     </row>
     <row r="39" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B39" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42022</v>
       </c>
       <c r="C39" s="18"/>
@@ -1852,7 +1862,7 @@
         <v>21.06451612903226</v>
       </c>
       <c r="F39" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>21.06451612903226</v>
       </c>
       <c r="I39" s="22">
@@ -1866,7 +1876,7 @@
     </row>
     <row r="40" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B40" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42023</v>
       </c>
       <c r="C40" s="18"/>
@@ -1878,7 +1888,7 @@
         <v>24.290322580645164</v>
       </c>
       <c r="F40" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>24.290322580645164</v>
       </c>
       <c r="I40" s="22">
@@ -1892,7 +1902,7 @@
     </row>
     <row r="41" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B41" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42024</v>
       </c>
       <c r="C41" s="18"/>
@@ -1904,7 +1914,7 @@
         <v>27.516129032258068</v>
       </c>
       <c r="F41" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>27.516129032258068</v>
       </c>
       <c r="I41" s="22">
@@ -1918,7 +1928,7 @@
     </row>
     <row r="42" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B42" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42025</v>
       </c>
       <c r="C42" s="18"/>
@@ -1930,7 +1940,7 @@
         <v>30.741935483870972</v>
       </c>
       <c r="F42" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>30.741935483870972</v>
       </c>
       <c r="I42" s="22">
@@ -1944,7 +1954,7 @@
     </row>
     <row r="43" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B43" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42026</v>
       </c>
       <c r="C43" s="18"/>
@@ -1956,7 +1966,7 @@
         <v>33.967741935483872</v>
       </c>
       <c r="F43" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>33.967741935483872</v>
       </c>
       <c r="I43" s="22">
@@ -1970,7 +1980,7 @@
     </row>
     <row r="44" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B44" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42027</v>
       </c>
       <c r="C44" s="18"/>
@@ -1982,7 +1992,7 @@
         <v>37.193548387096776</v>
       </c>
       <c r="F44" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>37.193548387096776</v>
       </c>
       <c r="I44" s="22">
@@ -1996,7 +2006,7 @@
     </row>
     <row r="45" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B45" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42028</v>
       </c>
       <c r="C45" s="18"/>
@@ -2008,7 +2018,7 @@
         <v>40.41935483870968</v>
       </c>
       <c r="F45" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>40.41935483870968</v>
       </c>
       <c r="I45" s="22">
@@ -2022,7 +2032,7 @@
     </row>
     <row r="46" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B46" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42029</v>
       </c>
       <c r="C46" s="25" t="s">
@@ -2036,7 +2046,7 @@
         <v>43.645161290322584</v>
       </c>
       <c r="F46" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-5.3548387096774164</v>
       </c>
       <c r="G46" s="28" t="s">
@@ -2053,7 +2063,7 @@
     </row>
     <row r="47" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B47" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42030</v>
       </c>
       <c r="C47" s="18"/>
@@ -2065,7 +2075,7 @@
         <v>-2.1290322580645133</v>
       </c>
       <c r="F47" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-2.1290322580645133</v>
       </c>
       <c r="I47" s="22">
@@ -2079,7 +2089,7 @@
     </row>
     <row r="48" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B48" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42031</v>
       </c>
       <c r="C48" s="18"/>
@@ -2091,7 +2101,7 @@
         <v>1.0967741935483897</v>
       </c>
       <c r="F48" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1.0967741935483897</v>
       </c>
       <c r="I48" s="22">
@@ -2105,7 +2115,7 @@
     </row>
     <row r="49" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B49" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42032</v>
       </c>
       <c r="C49" s="18"/>
@@ -2117,7 +2127,7 @@
         <v>4.3225806451612927</v>
       </c>
       <c r="F49" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>4.3225806451612927</v>
       </c>
       <c r="I49" s="22">
@@ -2131,7 +2141,7 @@
     </row>
     <row r="50" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B50" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42033</v>
       </c>
       <c r="C50" s="25" t="s">
@@ -2145,7 +2155,7 @@
         <v>7.5483870967741957</v>
       </c>
       <c r="F50" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>-2.4516129032258043</v>
       </c>
       <c r="I50" s="22">
@@ -2159,7 +2169,7 @@
     </row>
     <row r="51" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B51" s="24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42034</v>
       </c>
       <c r="C51" s="18"/>
@@ -2171,7 +2181,7 @@
         <v>0.77419354838709875</v>
       </c>
       <c r="F51" s="21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>0.77419354838709875</v>
       </c>
       <c r="I51" s="22">
@@ -2185,7 +2195,7 @@
     </row>
     <row r="52" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B52" s="36">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42035</v>
       </c>
       <c r="C52" s="31"/>
@@ -2197,7 +2207,7 @@
         <v>4.0000000000000018</v>
       </c>
       <c r="F52" s="34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>4.0000000000000018</v>
       </c>
       <c r="I52" s="22">
@@ -2210,10 +2220,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>96</v>
@@ -2229,6 +2239,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G25:G30"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B18:D19"/>
+    <mergeCell ref="B16:D17"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
@@ -2242,11 +2257,6 @@
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="G25:G30"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B18:D19"/>
-    <mergeCell ref="B16:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThanOrEqual">
@@ -2299,13 +2309,13 @@
         <v>42277</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -2325,28 +2335,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -2356,7 +2366,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -2447,48 +2457,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -3320,10 +3330,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -3407,13 +3417,13 @@
         <v>42308</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -3433,28 +3443,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -3464,7 +3474,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -3555,48 +3565,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -4428,10 +4438,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -4447,12 +4457,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="H8:H10"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
@@ -4463,6 +4467,12 @@
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
@@ -4515,13 +4525,13 @@
         <v>42338</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -4541,28 +4551,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -4572,7 +4582,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -4663,48 +4673,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -5536,10 +5546,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -5623,13 +5633,13 @@
         <v>42369</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -5649,28 +5659,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -5680,7 +5690,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -5771,48 +5781,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -6644,10 +6654,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -6663,12 +6673,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="B53:C53"/>
@@ -6679,6 +6683,12 @@
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="I20:J20"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
@@ -6696,17 +6706,188 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D8EF9C-FE92-DE42-8F65-6A896CD97F2B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>49</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <f>TYPE(D1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D2">
+        <v>1.3212999999999999</v>
+      </c>
+      <c r="E2" s="38">
+        <f t="shared" ref="E2:E22" si="0">TYPE(D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D3" s="39">
+        <v>1231</v>
+      </c>
+      <c r="E3" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D7" s="40">
+        <v>42006</v>
+      </c>
+      <c r="E7" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
+      <c r="D8" s="40">
+        <v>39114</v>
+      </c>
+      <c r="E8" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D11" t="e">
+        <f>Er</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E11" s="38">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D12">
+        <f>{1,2,3}</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="38">
+        <f>TYPE(D12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E13" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E14" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E15" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E16" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E17" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E18" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E19" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E20" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E21" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E22" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6751,13 +6932,13 @@
         <v>42063</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -6777,28 +6958,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -6808,7 +6989,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -6899,48 +7080,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -7772,10 +7953,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -7791,6 +7972,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="B53:C53"/>
@@ -7800,13 +7988,6 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThanOrEqual">
@@ -7859,13 +8040,13 @@
         <v>42094</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -7885,28 +8066,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -7916,7 +8097,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -8007,48 +8188,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -8880,10 +9061,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -8899,13 +9080,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:J10"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
@@ -8915,6 +9089,13 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:J10"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThanOrEqual">
@@ -8967,13 +9148,13 @@
         <v>42124</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -8993,28 +9174,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -9024,7 +9205,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -9115,48 +9296,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -9988,10 +10169,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -10007,22 +10188,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B16:D17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:J14"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B18:D19"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="E18:F19"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B16:D17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:J14"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThanOrEqual">
@@ -10075,13 +10256,13 @@
         <v>42155</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -10101,28 +10282,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -10132,7 +10313,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -10223,48 +10404,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -11096,10 +11277,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -11115,11 +11296,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="I20:J20"/>
@@ -11131,6 +11307,11 @@
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I11:J14"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThanOrEqual">
@@ -11183,13 +11364,13 @@
         <v>42185</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -11209,28 +11390,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -11240,7 +11421,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -11331,48 +11512,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -12204,10 +12385,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -12291,13 +12472,13 @@
         <v>42216</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -12317,28 +12498,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -12348,7 +12529,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -12439,48 +12620,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -13312,10 +13493,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>
@@ -13331,6 +13512,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="I20:J20"/>
@@ -13342,11 +13528,6 @@
     <mergeCell ref="E16:F17"/>
     <mergeCell ref="I8:J10"/>
     <mergeCell ref="I11:J14"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:F52">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThanOrEqual">
@@ -13399,13 +13580,13 @@
         <v>42247</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -13425,28 +13606,28 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="44"/>
+      <c r="E4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="H4" s="46" t="s">
+      <c r="F4" s="44"/>
+      <c r="H4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="E5" s="7"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
@@ -13456,7 +13637,7 @@
       <c r="H6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
@@ -13547,48 +13728,48 @@
       <c r="J14" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="49">
         <f>C14-F14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="49">
         <f>E16/(DAYS360(D2,F2)+1)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="39"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -14420,10 +14601,10 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="42"/>
+      <c r="C53" s="44"/>
       <c r="D53" s="35">
         <f>SUM(D22:D52)</f>
         <v>0</v>

</xml_diff>